<commit_message>
New profile added - Patient with Mandatory Identifier
New profile added into Diagnostic Report and Event Summary IGs.
</commit_message>
<xml_diff>
--- a/output/EventSummary/practitioner-dh-base-1.xlsx
+++ b/output/EventSummary/practitioner-dh-base-1.xlsx
@@ -9729,7 +9729,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="75" hidden="true">
+    <row r="75">
       <c r="A75" t="s" s="2">
         <v>317</v>
       </c>
@@ -9745,7 +9745,7 @@
         <v>42</v>
       </c>
       <c r="G75" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H75" t="s" s="2">
         <v>40</v>
@@ -9840,7 +9840,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76" hidden="true">
+    <row r="76">
       <c r="A76" t="s" s="2">
         <v>322</v>
       </c>
@@ -9856,7 +9856,7 @@
         <v>50</v>
       </c>
       <c r="G76" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H76" t="s" s="2">
         <v>40</v>
@@ -9949,7 +9949,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" hidden="true">
+    <row r="77">
       <c r="A77" t="s" s="2">
         <v>329</v>
       </c>
@@ -9965,7 +9965,7 @@
         <v>50</v>
       </c>
       <c r="G77" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H77" t="s" s="2">
         <v>40</v>
@@ -10060,7 +10060,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="78" hidden="true">
+    <row r="78">
       <c r="A78" t="s" s="2">
         <v>335</v>
       </c>
@@ -10076,7 +10076,7 @@
         <v>50</v>
       </c>
       <c r="G78" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H78" t="s" s="2">
         <v>40</v>

</xml_diff>

<commit_message>
Diagnostic Report and Event Summary IGs regenerated with updated profiles page & individual profile intro pages template
</commit_message>
<xml_diff>
--- a/output/EventSummary/practitioner-dh-base-1.xlsx
+++ b/output/EventSummary/practitioner-dh-base-1.xlsx
@@ -9729,7 +9729,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
         <v>317</v>
       </c>
@@ -9745,7 +9745,7 @@
         <v>42</v>
       </c>
       <c r="G75" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H75" t="s" s="2">
         <v>40</v>
@@ -9840,7 +9840,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
         <v>322</v>
       </c>
@@ -9856,7 +9856,7 @@
         <v>50</v>
       </c>
       <c r="G76" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H76" t="s" s="2">
         <v>40</v>
@@ -9949,7 +9949,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
         <v>329</v>
       </c>
@@ -9965,7 +9965,7 @@
         <v>50</v>
       </c>
       <c r="G77" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H77" t="s" s="2">
         <v>40</v>
@@ -10060,7 +10060,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
         <v>335</v>
       </c>
@@ -10076,7 +10076,7 @@
         <v>50</v>
       </c>
       <c r="G78" t="s" s="2">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H78" t="s" s="2">
         <v>40</v>

</xml_diff>